<commit_message>
SASI: Updated for Development
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RPAFNLD011\Documents\UiPath\FLCSMON_MANAGE_ORDERS_AND_ALLOCATION_CANCELLATION_PERFORMER\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RPAFNLD011\Desktop\Workspace_GitHub\FLCSMON_MANAGE_ORDERS_AND_ALLOCATION_CANCELLATION_PERFORMER\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -252,6 +252,80 @@
   </si>
   <si>
     <t xml:space="preserve">Hi Team&lt;br&gt;&lt;br&gt;Reason for rejections are not updated/fetched from SAP for the rejections in 1979 order for order ID &lt;OrderID&gt;. </t>
+  </si>
+  <si>
+    <t>SUB_Scenario1</t>
+  </si>
+  <si>
+    <t>Allocation Cancellation Bot - Manual Intervention Required - Delivery Note on Order &lt;O:Sales Document&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello,&lt;br&gt;&lt;br&gt;Please Have Delivery Note Removed: &lt;Delivery#&gt;. Once Delivery note is removed, please action this order with provided allocation changes
+</t>
+  </si>
+  <si>
+    <t>Body_Scenario1_Start</t>
+  </si>
+  <si>
+    <t>Body_Scenario1_End</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;br&gt;Thank You,</t>
+  </si>
+  <si>
+    <t>FLCSMON_Manage_Orders_Allocation_Cancellation_Distributor_BusinessNotificationEmails</t>
+  </si>
+  <si>
+    <t>SUB_ScenarioBulkCA</t>
+  </si>
+  <si>
+    <t>Body_ScenarioBulkCA_Start</t>
+  </si>
+  <si>
+    <t>Body_ScenarioBulkCA_End</t>
+  </si>
+  <si>
+    <t>CA Trader Bulk order adjustments - Order &lt;O:Sales Document&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello,&lt;br&gt;&lt;br&gt;Please note the below bulk orders were updated due to allocation. Please let us know if you see any issues with the product cancellation/reduction:&lt;br&gt;
+</t>
+  </si>
+  <si>
+    <t>FLCSMON_Manage_Orders_Allocation_Cancellation_Distributor_BusinessNotificationEmailsCC</t>
+  </si>
+  <si>
+    <t>SUB_ScenarioBulkEDC</t>
+  </si>
+  <si>
+    <t>Body_ScenarioBulkEDC_Start</t>
+  </si>
+  <si>
+    <t>Body_ScenarioBulkEDC_End</t>
+  </si>
+  <si>
+    <t>FLCSMON_Manage_Orders_Allocation_Cancellation_Distributor_BusinessNotificationEmailsEDC</t>
+  </si>
+  <si>
+    <t>FLCSMON_Manage_Orders_Allocation_Cancellation_Distributor_BusinessNotificationEmailsEDC_CC</t>
+  </si>
+  <si>
+    <t>US Bulk order adjustments - Order &lt;O:Sales Document&gt;</t>
+  </si>
+  <si>
+    <t>SUB_ScenarioBulkUS</t>
+  </si>
+  <si>
+    <t>Body_ScenarioBulkUS_Start</t>
+  </si>
+  <si>
+    <t>Body_ScenarioBulkUS_End</t>
+  </si>
+  <si>
+    <t>FLCSMON_Manage_Orders_Allocation_Cancellation_Distributor_BusinessNotificationEmailsUS</t>
+  </si>
+  <si>
+    <t>FLCSMON_Manage_Orders_Allocation_Cancellation_Distributor_BusinessNotificationEmailsUS_CC</t>
   </si>
 </sst>
 </file>
@@ -639,7 +713,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -780,24 +854,109 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="12" customHeight="1">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2946,7 +3105,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3081,12 +3240,72 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -4080,6 +4299,12 @@
     <hyperlink ref="C8" r:id="rId3"/>
     <hyperlink ref="C9" r:id="rId4"/>
     <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C10" r:id="rId6"/>
+    <hyperlink ref="C11" r:id="rId7"/>
+    <hyperlink ref="C12" r:id="rId8"/>
+    <hyperlink ref="C13" r:id="rId9"/>
+    <hyperlink ref="C14" r:id="rId10"/>
+    <hyperlink ref="C15" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>